<commit_message>
Update new version of Special Remake
</commit_message>
<xml_diff>
--- a/002-‘’Choco‘’SpecialRemake/002.BOM_CK_085_DCDC_Special_remake.xlsx
+++ b/002-‘’Choco‘’SpecialRemake/002.BOM_CK_085_DCDC_Special_remake.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="143">
   <si>
     <t>No.</t>
   </si>
@@ -115,6 +115,24 @@
     <t>5</t>
   </si>
   <si>
+    <t>1N5819WS</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SOD-323_L1.8-W1.3-LS2.5-RD</t>
+  </si>
+  <si>
+    <t>Hottech(合科泰)</t>
+  </si>
+  <si>
+    <t>C191023</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>2.4GHz</t>
   </si>
   <si>
@@ -133,7 +151,7 @@
     <t>C82891</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>22kΩ</t>
@@ -154,7 +172,7 @@
     <t>C25768</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>100kΩ</t>
@@ -169,7 +187,7 @@
     <t>C25741</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>2.2uH</t>
@@ -190,7 +208,7 @@
     <t>C5832372</t>
   </si>
   <si>
-    <t>9</t>
+    <t>10</t>
   </si>
   <si>
     <t>NH-B2020RGBA-HF</t>
@@ -208,7 +226,7 @@
     <t>C2874116</t>
   </si>
   <si>
-    <t>10</t>
+    <t>11</t>
   </si>
   <si>
     <t>TP4057-42-SOT26-R</t>
@@ -226,7 +244,7 @@
     <t>C12044</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>ESD5451N</t>
@@ -244,7 +262,25 @@
     <t>C2936977</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>AO3401A</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>SOT-23_L2.9-W1.3-P1.90-LS2.4-BR</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>C15127</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>4.7kΩ</t>
@@ -259,7 +295,22 @@
     <t>C25900</t>
   </si>
   <si>
-    <t>13</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>R9,VDG</t>
+  </si>
+  <si>
+    <t>0402WGF1002TCE</t>
+  </si>
+  <si>
+    <t>C25744</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
   <si>
     <t>2kΩ</t>
@@ -274,7 +325,7 @@
     <t>C4109</t>
   </si>
   <si>
-    <t>14</t>
+    <t>17</t>
   </si>
   <si>
     <t>5.1kΩ</t>
@@ -289,7 +340,7 @@
     <t>C25905</t>
   </si>
   <si>
-    <t>15</t>
+    <t>18</t>
   </si>
   <si>
     <t>1kΩ</t>
@@ -304,7 +355,7 @@
     <t>C11702</t>
   </si>
   <si>
-    <t>16</t>
+    <t>19</t>
   </si>
   <si>
     <t>SSSS811101</t>
@@ -322,7 +373,7 @@
     <t>C109335</t>
   </si>
   <si>
-    <t>17</t>
+    <t>20</t>
   </si>
   <si>
     <t>M3406-ADJ</t>
@@ -340,7 +391,7 @@
     <t>C83224</t>
   </si>
   <si>
-    <t>18</t>
+    <t>21</t>
   </si>
   <si>
     <t>CH340X</t>
@@ -358,7 +409,7 @@
     <t>C3035748</t>
   </si>
   <si>
-    <t>19</t>
+    <t>22</t>
   </si>
   <si>
     <t>TYPE-C 16PIN 2MD(073)</t>
@@ -376,22 +427,7 @@
     <t>C2765186</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
-    <t>VDG</t>
-  </si>
-  <si>
-    <t>0402WGF1002TCE</t>
-  </si>
-  <si>
-    <t>C25744</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>23</t>
   </si>
   <si>
     <t>47kΩ</t>
@@ -780,7 +816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -966,16 +1002,16 @@
         <v>36</v>
       </c>
       <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
       </c>
       <c r="J6" t="s">
         <v>18</v>
@@ -983,31 +1019,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>45</v>
-      </c>
-      <c r="I7" t="s">
-        <v>46</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -1015,31 +1051,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J8" t="s">
         <v>18</v>
@@ -1047,31 +1083,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>54</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
       </c>
       <c r="G9" t="s">
         <v>56</v>
       </c>
       <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
         <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>58</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
@@ -1079,25 +1115,25 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>61</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
         <v>62</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
       </c>
       <c r="H10" t="s">
         <v>63</v>
@@ -1178,7 +1214,7 @@
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>78</v>
@@ -1187,19 +1223,19 @@
         <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
         <v>78</v>
       </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J13" t="s">
         <v>18</v>
@@ -1207,31 +1243,31 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
         <v>84</v>
       </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" t="s">
-        <v>85</v>
-      </c>
       <c r="H14" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J14" t="s">
         <v>18</v>
@@ -1239,31 +1275,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
@@ -1271,31 +1307,31 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J16" t="s">
         <v>18</v>
@@ -1303,31 +1339,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
         <v>100</v>
       </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H17" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="I17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J17" t="s">
         <v>18</v>
@@ -1335,28 +1371,28 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
         <v>105</v>
       </c>
-      <c r="E18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" t="s">
-        <v>28</v>
-      </c>
       <c r="G18" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="I18" t="s">
         <v>108</v>
@@ -1379,19 +1415,19 @@
         <v>111</v>
       </c>
       <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
         <v>112</v>
       </c>
-      <c r="F19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" t="s">
-        <v>110</v>
-      </c>
       <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" t="s">
         <v>113</v>
-      </c>
-      <c r="I19" t="s">
-        <v>114</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
@@ -1399,31 +1435,31 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>115</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>116</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>117</v>
-      </c>
-      <c r="E20" t="s">
-        <v>118</v>
       </c>
       <c r="F20" t="s">
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" t="s">
         <v>119</v>
-      </c>
-      <c r="I20" t="s">
-        <v>120</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
@@ -1431,28 +1467,28 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
         <v>121</v>
       </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>122</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>123</v>
       </c>
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" t="s">
         <v>124</v>
-      </c>
-      <c r="H21" t="s">
-        <v>45</v>
       </c>
       <c r="I21" t="s">
         <v>125</v>
@@ -1475,26 +1511,90 @@
         <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="F22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" t="s">
         <v>127</v>
       </c>
-      <c r="G22" t="s">
-        <v>129</v>
-      </c>
       <c r="H22" t="s">
-        <v>45</v>
+        <v>130</v>
       </c>
       <c r="I22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" t="s">
+        <v>137</v>
+      </c>
+      <c r="J23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" t="s">
+        <v>141</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" t="s">
+        <v>142</v>
+      </c>
+      <c r="J24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>